<commit_message>
- Better output for hkpk Signed-off-by: Shahidul Islam <shahid.sm35@gmail.com>
</commit_message>
<xml_diff>
--- a/data/database/TimeUpdate.xlsx
+++ b/data/database/TimeUpdate.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="0" windowWidth="19380" windowHeight="8055" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="19380" windowHeight="8055" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ipknot_cro" sheetId="1" r:id="rId1"/>
     <sheet name="hk_short_cro" sheetId="2" r:id="rId2"/>
     <sheet name="hk_long_cro" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="ipknot_knotty" sheetId="5" r:id="rId5"/>
-    <sheet name="hk_short_knotty" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId7"/>
-    <sheet name="hk_long_knotty" sheetId="7" r:id="rId8"/>
+    <sheet name="dk_cro_and_knotty" sheetId="9" r:id="rId5"/>
+    <sheet name="ipknot_knotty" sheetId="5" r:id="rId6"/>
+    <sheet name="hk_short_knotty" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="hk_long_knotty" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="120">
   <si>
     <t>Column1</t>
   </si>
@@ -329,6 +330,69 @@
   <si>
     <t>**</t>
   </si>
+  <si>
+    <t>RF00010_RNAseP.txt</t>
+  </si>
+  <si>
+    <t>RF00025_Telomerase_Cil.txt</t>
+  </si>
+  <si>
+    <t>RF00023_tmRNA.txt</t>
+  </si>
+  <si>
+    <t>RF00094_HDV.txt</t>
+  </si>
+  <si>
+    <t>RF00114_S15.txt</t>
+  </si>
+  <si>
+    <t>RF00162_SAMI.txt</t>
+  </si>
+  <si>
+    <t>RF00165_BCV.txt</t>
+  </si>
+  <si>
+    <t>RF00234_glmS.txt</t>
+  </si>
+  <si>
+    <t>RF00209_CSFV.txt</t>
+  </si>
+  <si>
+    <t>RF00290_BaMV.txt</t>
+  </si>
+  <si>
+    <t>RF00499_HPeV1.txt</t>
+  </si>
+  <si>
+    <t>RF00507_SARSCoV.txt</t>
+  </si>
+  <si>
+    <t>RF01087_repZ.txt</t>
+  </si>
+  <si>
+    <t>RF01840_VMV.txt</t>
+  </si>
+  <si>
+    <t>RF00458_IRES_PSIV.txt</t>
+  </si>
+  <si>
+    <t>RF00522_preQ1.txt</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Cro</t>
+  </si>
+  <si>
+    <t>Knotty</t>
+  </si>
+  <si>
+    <t>Knotty2</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
@@ -588,7 +652,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -898,6 +968,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:E18" totalsRowShown="0">
+  <autoFilter ref="B1:E18"/>
+  <sortState ref="B2:D17">
+    <sortCondition ref="B1:B18"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Seq"/>
+    <tableColumn id="2" name="Cro" dataDxfId="1"/>
+    <tableColumn id="4" name="Knotty" dataDxfId="0"/>
+    <tableColumn id="3" name="Knotty2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:B239" totalsRowShown="0">
   <autoFilter ref="A1:B239"/>
   <sortState ref="A2:B239">
@@ -911,25 +997,25 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="E1:G170" totalsRowCount="1" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="E1:G170" totalsRowCount="1" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="E1:G169"/>
   <sortState ref="E2:F169">
     <sortCondition ref="E1:E169"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" name="Column12" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="1" name="Column1" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Column12" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>Table10[[#This Row],[Column2]]/1000</calculatedColumnFormula>
       <totalsRowFormula>AVERAGE(F1:F169)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="Column2" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Column2" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:C79" totalsRowShown="0">
   <autoFilter ref="A1:C79"/>
   <sortState ref="A2:C79">
@@ -938,7 +1024,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3" dataDxfId="1">
+    <tableColumn id="3" name="Column3" dataDxfId="3">
       <calculatedColumnFormula>Table8[[#This Row],[Column2]]/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -946,7 +1032,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C11" totalsRowShown="0">
   <autoFilter ref="A1:C11"/>
   <sortState ref="A2:C10">
@@ -954,7 +1040,7 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="3" name="Column12" dataDxfId="0">
+    <tableColumn id="3" name="Column12" dataDxfId="2">
       <calculatedColumnFormula>Table9[[#This Row],[Column2]]/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Column2"/>
@@ -9937,9 +10023,346 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="4" width="11" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="7">
+        <v>104.14</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="7">
+        <v>26.74</v>
+      </c>
+      <c r="D4" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>447.58600000000001</v>
+      </c>
+      <c r="E4">
+        <v>447586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="D5" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>24.385000000000002</v>
+      </c>
+      <c r="E5">
+        <v>24385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="D6" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>10.663</v>
+      </c>
+      <c r="E6">
+        <v>10663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.23</v>
+      </c>
+      <c r="D7" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>31.239000000000001</v>
+      </c>
+      <c r="E7">
+        <v>31239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="D8" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>4.8040000000000003</v>
+      </c>
+      <c r="E8">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="7">
+        <v>18.93</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4.91</v>
+      </c>
+      <c r="D10" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>371.303</v>
+      </c>
+      <c r="E10">
+        <v>371303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="D11" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>950.60799999999995</v>
+      </c>
+      <c r="E11">
+        <v>950608</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="7">
+        <v>17.87</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="7">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="D13" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>97.549000000000007</v>
+      </c>
+      <c r="E13">
+        <v>97549</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2.67</v>
+      </c>
+      <c r="D14" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>18.09</v>
+      </c>
+      <c r="E14">
+        <v>18090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="D15" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="E15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1.37</v>
+      </c>
+      <c r="D16" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>301.76400000000001</v>
+      </c>
+      <c r="E16">
+        <v>301764</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="D17" s="7">
+        <f>Table1[[#This Row],[Knotty2]]/1000</f>
+        <v>6.6</v>
+      </c>
+      <c r="E17">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="7">
+        <f>AVERAGE(C2:C17)</f>
+        <v>12.170624999999998</v>
+      </c>
+      <c r="D18" s="7">
+        <f>SUM(D2:D17)/12</f>
+        <v>188.73325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A144" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J169" sqref="J169"/>
     </sheetView>
   </sheetViews>
@@ -14745,7 +15168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C79"/>
   <sheetViews>
@@ -15714,7 +16137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E169"/>
   <sheetViews>
@@ -17112,7 +17535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>

</xml_diff>